<commit_message>
Made a minor change to GSX.py. Uploaded new results excel sheets. Uploaded last week's dark pool data feed.
</commit_message>
<xml_diff>
--- a/BB Alert Result Statistics.xlsx
+++ b/BB Alert Result Statistics.xlsx
@@ -1,93 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/swiftteamsix/Dropbox/Business/Yolo Capital/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90DAFFC1-B037-9440-87B7-88FF800A3597}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="41640" yWindow="20380" windowWidth="35160" windowHeight="22820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t>%GAIN</t>
-  </si>
-  <si>
-    <t>count</t>
-  </si>
-  <si>
-    <t>max</t>
-  </si>
-  <si>
-    <t>mean</t>
-  </si>
-  <si>
-    <t>DETAILS</t>
-  </si>
-  <si>
-    <t>Large_Bullish</t>
-  </si>
-  <si>
-    <t>Rapidfire_Bullish</t>
-  </si>
-  <si>
-    <t>Repeater_Bearish</t>
-  </si>
-  <si>
-    <t>Repeater_Bullish</t>
-  </si>
-  <si>
-    <t>Roulette_Bearish</t>
-  </si>
-  <si>
-    <t>Roulette_Bullish</t>
-  </si>
-  <si>
-    <t>Steady_Bullish</t>
-  </si>
-  <si>
-    <t>Swift_Bullish</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -96,46 +46,54 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="2">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -423,162 +381,186 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4">
-        <v>147</v>
-      </c>
-      <c r="C4">
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr"/>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>%GAIN</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="n"/>
+      <c r="D1" s="1" t="n"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr"/>
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>count</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>max</t>
+        </is>
+      </c>
+      <c r="D2" s="1" t="inlineStr">
+        <is>
+          <t>mean</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>DETAILS</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Large_Bullish</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>9</v>
+      </c>
+      <c r="C4" t="n">
         <v>19.23</v>
       </c>
-      <c r="D4">
-        <v>10.331428571428569</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5">
-        <v>273</v>
-      </c>
-      <c r="C5">
+      <c r="D4" t="n">
+        <v>8.217777777777776</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Rapidfire_Bullish</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>16</v>
+      </c>
+      <c r="C5" t="n">
         <v>208.11</v>
       </c>
-      <c r="D5">
-        <v>44.684615384615341</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6">
-        <v>609</v>
-      </c>
-      <c r="C6">
+      <c r="D5" t="n">
+        <v>43.0575</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Repeater_Bearish</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>39</v>
+      </c>
+      <c r="C6" t="n">
         <v>352.38</v>
       </c>
-      <c r="D6">
-        <v>52.101379310344981</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7">
-        <v>945</v>
-      </c>
-      <c r="C7">
-        <v>186.49</v>
-      </c>
-      <c r="D7">
-        <v>28.640666666666728</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8">
-        <v>1155</v>
-      </c>
-      <c r="C8">
+      <c r="D6" t="n">
+        <v>56.06564102564101</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Repeater_Bullish</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>71</v>
+      </c>
+      <c r="C7" t="n">
+        <v>215.15</v>
+      </c>
+      <c r="D7" t="n">
+        <v>32.06704225352112</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Roulette_Bearish</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>77</v>
+      </c>
+      <c r="C8" t="n">
         <v>1028.21</v>
       </c>
-      <c r="D8">
-        <v>59.065636363636372</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9">
-        <v>945</v>
-      </c>
-      <c r="C9">
-        <v>318.35000000000002</v>
-      </c>
-      <c r="D9">
-        <v>42.573555555555629</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10">
-        <v>441</v>
-      </c>
-      <c r="C10">
-        <v>80.56</v>
-      </c>
-      <c r="D10">
-        <v>30.672380952381001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11">
-        <v>315</v>
-      </c>
-      <c r="C11">
+      <c r="D8" t="n">
+        <v>50.75467532467533</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>Roulette_Bullish</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>58</v>
+      </c>
+      <c r="C9" t="n">
+        <v>318.35</v>
+      </c>
+      <c r="D9" t="n">
+        <v>50.40137931034482</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>Steady_Bullish</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>28</v>
+      </c>
+      <c r="C10" t="n">
+        <v>90.91</v>
+      </c>
+      <c r="D10" t="n">
+        <v>31.71571428571428</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>Swift_Bullish</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>21</v>
+      </c>
+      <c r="C11" t="n">
         <v>159.41</v>
       </c>
-      <c r="D11">
-        <v>42.768666666666661</v>
+      <c r="D11" t="n">
+        <v>38.07952380952381</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:D1"/>
   </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated results of GSX dark pool
</commit_message>
<xml_diff>
--- a/BB Alert Result Statistics.xlsx
+++ b/BB Alert Result Statistics.xlsx
@@ -1,43 +1,93 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/swiftteamsix/Dropbox/Business/Yolo Capital/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D907664-0221-A14F-B844-1FDFAD020617}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="720" yWindow="460" windowWidth="76080" windowHeight="42740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+  <si>
+    <t>%GAIN</t>
+  </si>
+  <si>
+    <t>count</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>DETAILS</t>
+  </si>
+  <si>
+    <t>Large_Bullish</t>
+  </si>
+  <si>
+    <t>Rapidfire_Bullish</t>
+  </si>
+  <si>
+    <t>Repeater_Bearish</t>
+  </si>
+  <si>
+    <t>Repeater_Bullish</t>
+  </si>
+  <si>
+    <t>Roulette_Bearish</t>
+  </si>
+  <si>
+    <t>Roulette_Bullish</t>
+  </si>
+  <si>
+    <t>Steady_Bullish</t>
+  </si>
+  <si>
+    <t>Swift_Bullish</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -46,54 +96,46 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -381,186 +423,157 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr"/>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>%GAIN</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="n"/>
-      <c r="D1" s="1" t="n"/>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="inlineStr"/>
-      <c r="B2" s="1" t="inlineStr">
-        <is>
-          <t>count</t>
-        </is>
-      </c>
-      <c r="C2" s="1" t="inlineStr">
-        <is>
-          <t>max</t>
-        </is>
-      </c>
-      <c r="D2" s="1" t="inlineStr">
-        <is>
-          <t>mean</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>DETAILS</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>Large_Bullish</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>17</v>
+      </c>
+      <c r="C4">
+        <v>25.62</v>
+      </c>
+      <c r="D4">
+        <v>7.8729411764705883</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>77</v>
+      </c>
+      <c r="C5">
+        <v>260.87</v>
+      </c>
+      <c r="D5">
+        <v>48.817142857142848</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>97</v>
+      </c>
+      <c r="C6">
+        <v>629.01</v>
+      </c>
+      <c r="D6">
+        <v>64.565979381443327</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>305</v>
+      </c>
+      <c r="C7">
+        <v>479.23</v>
+      </c>
+      <c r="D7">
+        <v>41.751934426229553</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="n">
-        <v>19.23</v>
-      </c>
-      <c r="D4" t="n">
-        <v>8.217777777777776</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>Rapidfire_Bullish</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>16</v>
-      </c>
-      <c r="C5" t="n">
-        <v>208.11</v>
-      </c>
-      <c r="D5" t="n">
-        <v>43.0575</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>Repeater_Bearish</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>39</v>
-      </c>
-      <c r="C6" t="n">
-        <v>352.38</v>
-      </c>
-      <c r="D6" t="n">
-        <v>56.06564102564101</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="inlineStr">
-        <is>
-          <t>Repeater_Bullish</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>71</v>
-      </c>
-      <c r="C7" t="n">
-        <v>215.15</v>
-      </c>
-      <c r="D7" t="n">
-        <v>32.06704225352112</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t>Roulette_Bearish</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>77</v>
-      </c>
-      <c r="C8" t="n">
+      <c r="B8">
+        <v>238</v>
+      </c>
+      <c r="C8">
         <v>1028.21</v>
       </c>
-      <c r="D8" t="n">
-        <v>50.75467532467533</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="inlineStr">
-        <is>
-          <t>Roulette_Bullish</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>58</v>
-      </c>
-      <c r="C9" t="n">
-        <v>318.35</v>
-      </c>
-      <c r="D9" t="n">
-        <v>50.40137931034482</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="inlineStr">
-        <is>
-          <t>Steady_Bullish</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>28</v>
-      </c>
-      <c r="C10" t="n">
-        <v>90.91</v>
-      </c>
-      <c r="D10" t="n">
-        <v>31.71571428571428</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="inlineStr">
-        <is>
-          <t>Swift_Bullish</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>21</v>
-      </c>
-      <c r="C11" t="n">
-        <v>159.41</v>
-      </c>
-      <c r="D11" t="n">
-        <v>38.07952380952381</v>
+      <c r="D8">
+        <v>43.84050420168068</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>185</v>
+      </c>
+      <c r="C9">
+        <v>318.35000000000002</v>
+      </c>
+      <c r="D9">
+        <v>39.667945945945938</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10">
+        <v>94</v>
+      </c>
+      <c r="C10">
+        <v>518.17999999999995</v>
+      </c>
+      <c r="D10">
+        <v>37.01351063829788</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <v>78</v>
+      </c>
+      <c r="C11">
+        <v>215.38</v>
+      </c>
+      <c r="D11">
+        <v>36.283333333333353</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:D1"/>
   </mergeCells>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated GSX results spreadsheet and BB Alert Result Statistics
</commit_message>
<xml_diff>
--- a/BB Alert Result Statistics.xlsx
+++ b/BB Alert Result Statistics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/swiftteamsix/Dropbox/Business/Yolo Capital/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D907664-0221-A14F-B844-1FDFAD020617}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DE0A116-B6A1-6C4B-9029-402D100A7FAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="720" yWindow="460" windowWidth="76080" windowHeight="42740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -426,11 +426,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:D6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -463,13 +468,13 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C4">
-        <v>25.62</v>
+        <v>33.35</v>
       </c>
       <c r="D4">
-        <v>7.8729411764705883</v>
+        <v>8.8309523809523807</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -477,13 +482,13 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="C5">
-        <v>260.87</v>
+        <v>586.27</v>
       </c>
       <c r="D5">
-        <v>48.817142857142848</v>
+        <v>55.85230769230769</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -491,13 +496,13 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="C6">
         <v>629.01</v>
       </c>
       <c r="D6">
-        <v>64.565979381443327</v>
+        <v>64.342233009708764</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -505,13 +510,13 @@
         <v>8</v>
       </c>
       <c r="B7">
-        <v>305</v>
+        <v>338</v>
       </c>
       <c r="C7">
-        <v>479.23</v>
+        <v>507.5</v>
       </c>
       <c r="D7">
-        <v>41.751934426229553</v>
+        <v>43.209171597633173</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -519,13 +524,13 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>238</v>
+        <v>272</v>
       </c>
       <c r="C8">
         <v>1028.21</v>
       </c>
       <c r="D8">
-        <v>43.84050420168068</v>
+        <v>43.639301470588229</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -533,13 +538,13 @@
         <v>10</v>
       </c>
       <c r="B9">
-        <v>185</v>
+        <v>198</v>
       </c>
       <c r="C9">
         <v>318.35000000000002</v>
       </c>
       <c r="D9">
-        <v>39.667945945945938</v>
+        <v>38.082373737373729</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -547,13 +552,13 @@
         <v>11</v>
       </c>
       <c r="B10">
-        <v>94</v>
+        <v>107</v>
       </c>
       <c r="C10">
         <v>518.17999999999995</v>
       </c>
       <c r="D10">
-        <v>37.01351063829788</v>
+        <v>36.638504672897191</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -561,13 +566,13 @@
         <v>12</v>
       </c>
       <c r="B11">
-        <v>78</v>
+        <v>95</v>
       </c>
       <c r="C11">
         <v>215.38</v>
       </c>
       <c r="D11">
-        <v>36.283333333333353</v>
+        <v>39.774947368421053</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated GSX results spreadsheet and BB Alert Result Statistics 7/19
</commit_message>
<xml_diff>
--- a/BB Alert Result Statistics.xlsx
+++ b/BB Alert Result Statistics.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/swiftteamsix/Dropbox/Business/Yolo Capital/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DE0A116-B6A1-6C4B-9029-402D100A7FAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{511DDF53-EEA1-4C45-8E3A-2F9967951F60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="720" yWindow="460" windowWidth="76080" windowHeight="42740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -426,8 +426,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:D6"/>
+    <sheetView tabSelected="1" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -468,13 +468,13 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C4">
-        <v>33.35</v>
+        <v>39.409999999999997</v>
       </c>
       <c r="D4">
-        <v>8.8309523809523807</v>
+        <v>9.8000000000000007</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -482,13 +482,13 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="C5">
         <v>586.27</v>
       </c>
       <c r="D5">
-        <v>55.85230769230769</v>
+        <v>55.020792079207922</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -496,13 +496,13 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="C6">
         <v>629.01</v>
       </c>
       <c r="D6">
-        <v>64.342233009708764</v>
+        <v>62.776481481481497</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -510,13 +510,13 @@
         <v>8</v>
       </c>
       <c r="B7">
-        <v>338</v>
+        <v>375</v>
       </c>
       <c r="C7">
         <v>507.5</v>
       </c>
       <c r="D7">
-        <v>43.209171597633173</v>
+        <v>41.899120000000032</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -524,13 +524,13 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>272</v>
+        <v>297</v>
       </c>
       <c r="C8">
         <v>1028.21</v>
       </c>
       <c r="D8">
-        <v>43.639301470588229</v>
+        <v>47.807306397306391</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -538,13 +538,13 @@
         <v>10</v>
       </c>
       <c r="B9">
-        <v>198</v>
+        <v>221</v>
       </c>
       <c r="C9">
         <v>318.35000000000002</v>
       </c>
       <c r="D9">
-        <v>38.082373737373729</v>
+        <v>38.557828054298618</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -552,13 +552,13 @@
         <v>11</v>
       </c>
       <c r="B10">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="C10">
         <v>518.17999999999995</v>
       </c>
       <c r="D10">
-        <v>36.638504672897191</v>
+        <v>40.057457627118623</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -566,13 +566,13 @@
         <v>12</v>
       </c>
       <c r="B11">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="C11">
         <v>215.38</v>
       </c>
       <c r="D11">
-        <v>39.774947368421053</v>
+        <v>39.846666666666657</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated GSX results spreadsheet and BB Alert Result Statistics 7/26
</commit_message>
<xml_diff>
--- a/BB Alert Result Statistics.xlsx
+++ b/BB Alert Result Statistics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/swiftteamsix/Dropbox/Business/Yolo Capital/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{511DDF53-EEA1-4C45-8E3A-2F9967951F60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{007C35E0-6153-BF4D-BBD3-58CB2DB312F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="720" yWindow="460" windowWidth="76080" windowHeight="42740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -426,9 +426,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="240" zoomScaleNormal="240" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -482,13 +480,13 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="C5">
         <v>586.27</v>
       </c>
       <c r="D5">
-        <v>55.020792079207922</v>
+        <v>53.668545454545459</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -496,13 +494,13 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="C6">
         <v>629.01</v>
       </c>
       <c r="D6">
-        <v>62.776481481481497</v>
+        <v>60.574649122807052</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -510,13 +508,13 @@
         <v>8</v>
       </c>
       <c r="B7">
-        <v>375</v>
+        <v>396</v>
       </c>
       <c r="C7">
         <v>507.5</v>
       </c>
       <c r="D7">
-        <v>41.899120000000032</v>
+        <v>41.434065656565693</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -524,13 +522,13 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>297</v>
+        <v>308</v>
       </c>
       <c r="C8">
         <v>1028.21</v>
       </c>
       <c r="D8">
-        <v>47.807306397306391</v>
+        <v>46.914610389610367</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -538,13 +536,13 @@
         <v>10</v>
       </c>
       <c r="B9">
-        <v>221</v>
+        <v>234</v>
       </c>
       <c r="C9">
-        <v>318.35000000000002</v>
+        <v>416.85</v>
       </c>
       <c r="D9">
-        <v>38.557828054298618</v>
+        <v>41.268547008546989</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -552,13 +550,13 @@
         <v>11</v>
       </c>
       <c r="B10">
-        <v>118</v>
+        <v>132</v>
       </c>
       <c r="C10">
         <v>518.17999999999995</v>
       </c>
       <c r="D10">
-        <v>40.057457627118623</v>
+        <v>38.441666666666663</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -566,13 +564,13 @@
         <v>12</v>
       </c>
       <c r="B11">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="C11">
         <v>215.38</v>
       </c>
       <c r="D11">
-        <v>39.846666666666657</v>
+        <v>39.052321428571418</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated GSX results spreadsheet and BB Alert Result Statistics 8/28
</commit_message>
<xml_diff>
--- a/BB Alert Result Statistics.xlsx
+++ b/BB Alert Result Statistics.xlsx
@@ -1,93 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/swiftteamsix/Dropbox/Business/Yolo Capital/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{007C35E0-6153-BF4D-BBD3-58CB2DB312F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="460" windowWidth="76080" windowHeight="42740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t>%GAIN</t>
-  </si>
-  <si>
-    <t>count</t>
-  </si>
-  <si>
-    <t>max</t>
-  </si>
-  <si>
-    <t>mean</t>
-  </si>
-  <si>
-    <t>DETAILS</t>
-  </si>
-  <si>
-    <t>Large_Bullish</t>
-  </si>
-  <si>
-    <t>Rapidfire_Bullish</t>
-  </si>
-  <si>
-    <t>Repeater_Bearish</t>
-  </si>
-  <si>
-    <t>Repeater_Bullish</t>
-  </si>
-  <si>
-    <t>Roulette_Bearish</t>
-  </si>
-  <si>
-    <t>Roulette_Bullish</t>
-  </si>
-  <si>
-    <t>Steady_Bullish</t>
-  </si>
-  <si>
-    <t>Swift_Bullish</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -96,46 +46,122 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -423,154 +449,180 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="240" zoomScaleNormal="240" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4">
-        <v>23</v>
-      </c>
-      <c r="C4">
-        <v>39.409999999999997</v>
-      </c>
-      <c r="D4">
-        <v>9.8000000000000007</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5">
-        <v>110</v>
-      </c>
-      <c r="C5">
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr"/>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>%GAIN</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="n"/>
+      <c r="D1" s="1" t="n"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr"/>
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>count</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>max</t>
+        </is>
+      </c>
+      <c r="D2" s="1" t="inlineStr">
+        <is>
+          <t>mean</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>DETAILS</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Large_Bullish</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>29</v>
+      </c>
+      <c r="C4" t="n">
+        <v>86.03</v>
+      </c>
+      <c r="D4" t="n">
+        <v>14.35448275862069</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Rapidfire_Bullish</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>112</v>
+      </c>
+      <c r="C5" t="n">
         <v>586.27</v>
       </c>
-      <c r="D5">
-        <v>53.668545454545459</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6">
-        <v>114</v>
-      </c>
-      <c r="C6">
+      <c r="D5" t="n">
+        <v>53.22151785714287</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Repeater_Bearish</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>116</v>
+      </c>
+      <c r="C6" t="n">
         <v>629.01</v>
       </c>
-      <c r="D6">
-        <v>60.574649122807052</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7">
-        <v>396</v>
-      </c>
-      <c r="C7">
+      <c r="D6" t="n">
+        <v>59.82534482758623</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Repeater_Bullish</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>404</v>
+      </c>
+      <c r="C7" t="n">
         <v>507.5</v>
       </c>
-      <c r="D7">
-        <v>41.434065656565693</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8">
-        <v>308</v>
-      </c>
-      <c r="C8">
+      <c r="D7" t="n">
+        <v>42.09767326732674</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Roulette_Bearish</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>311</v>
+      </c>
+      <c r="C8" t="n">
         <v>1028.21</v>
       </c>
-      <c r="D8">
-        <v>46.914610389610367</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9">
-        <v>234</v>
-      </c>
-      <c r="C9">
-        <v>416.85</v>
-      </c>
-      <c r="D9">
-        <v>41.268547008546989</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10">
-        <v>132</v>
-      </c>
-      <c r="C10">
-        <v>518.17999999999995</v>
-      </c>
-      <c r="D10">
-        <v>38.441666666666663</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11">
-        <v>112</v>
-      </c>
-      <c r="C11">
+      <c r="D8" t="n">
+        <v>46.55363344051445</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>Roulette_Bullish</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>241</v>
+      </c>
+      <c r="C9" t="n">
+        <v>702.4</v>
+      </c>
+      <c r="D9" t="n">
+        <v>43.94037344398338</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>Steady_Bullish</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>141</v>
+      </c>
+      <c r="C10" t="n">
+        <v>518.1799999999999</v>
+      </c>
+      <c r="D10" t="n">
+        <v>39.4386524822695</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>Swift_Bullish</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>116</v>
+      </c>
+      <c r="C11" t="n">
         <v>215.38</v>
       </c>
-      <c r="D11">
-        <v>39.052321428571418</v>
+      <c r="D11" t="n">
+        <v>38.2476724137931</v>
       </c>
     </row>
   </sheetData>

</xml_diff>